<commit_message>
Integrated all sensors with BLE, polling data with their correct size, missing: time, and comfort
</commit_message>
<xml_diff>
--- a/Docs/UUID Comfort Sensor.xlsx
+++ b/Docs/UUID Comfort Sensor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Exo-sensing\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A066F4CF-38FB-4C46-A968-DC680A6B5B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B3681C-D3E5-45CA-94AF-4751B32EF73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0085F328-8D57-4202-B787-25C916C50B19}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{0085F328-8D57-4202-B787-25C916C50B19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="76">
   <si>
     <t>[Service] Characteristic Value
 |- Descriptors</t>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>"Fuzzy Comfort"</t>
+  </si>
+  <si>
+    <t>HTS221 Humidity Reading</t>
   </si>
 </sst>
 </file>
@@ -713,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B2AAA8C-E17D-48BF-AE1C-CFD5917FB803}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +856,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>7</v>

</xml_diff>